<commit_message>
[update] 更新 SDK 版本为 v1.1
同步输出 WiFi 版本 1.0.5
同步输出 BLE 版本 1.0.2

更细 CHANGELOG.md

Signed-off-by: MurphyZhao <d2014zjt@163.com>
</commit_message>
<xml_diff>
--- a/doc/LN882H分区地址计算器.xlsx
+++ b/doc/LN882H分区地址计算器.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,16 +78,16 @@
     <t>PART_TAB</t>
   </si>
   <si>
-    <t>NVDS</t>
-  </si>
-  <si>
     <t>APP</t>
   </si>
   <si>
     <t>OTA</t>
   </si>
   <si>
-    <t>&gt;=APP分区的65%</t>
+    <t>&gt;=APP分区的60%</t>
+  </si>
+  <si>
+    <t>NVDS</t>
   </si>
   <si>
     <t>KV</t>
@@ -104,11 +104,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -153,6 +153,37 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -161,14 +192,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,6 +213,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -189,15 +236,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -211,9 +252,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,22 +283,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -251,14 +290,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -267,37 +298,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color rgb="FF00B050"/>
       <name val="新宋体"/>
@@ -337,31 +337,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,151 +517,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,6 +692,45 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -711,40 +750,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -776,17 +787,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -801,10 +801,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -813,137 +813,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1007,18 +1007,18 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1037,26 +1037,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1119,8 +1113,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="0001FF72"/>
       <color rgb="005FFFA3"/>
-      <color rgb="0001FF72"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1420,17 +1414,17 @@
   <sheetPr/>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="23.7777777777778" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.775" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.6666666666667" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.5555555555556" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.2222222222222" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.7777777777778" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.5583333333333" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.225" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.775" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.6666666666667" style="3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1444,14 +1438,14 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" ht="22.95" spans="1:6">
+    <row r="2" ht="23.25" spans="1:6">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" ht="18.15" spans="1:2">
+    <row r="3" ht="19.5" spans="1:2">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
@@ -1459,7 +1453,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="4" ht="15.15"/>
+    <row r="4" ht="14.25"/>
     <row r="5" spans="1:6">
       <c r="A5" s="10" t="s">
         <v>2</v>
@@ -1488,16 +1482,16 @@
         <v>0</v>
       </c>
       <c r="C6" s="15" t="str">
-        <f>"0x"&amp;RIGHT("00000000"&amp;DEC2HEX(B6),8)</f>
+        <f t="shared" ref="C6:C12" si="0">"0x"&amp;RIGHT("00000000"&amp;DEC2HEX(B6),8)</f>
         <v>0x00000000</v>
       </c>
       <c r="D6" s="15">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="17">
-        <f t="shared" ref="F6:F12" si="0">D6/4</f>
-        <v>9</v>
+        <f t="shared" ref="F6:F12" si="1">D6/4</f>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1505,19 +1499,19 @@
         <v>9</v>
       </c>
       <c r="B7" s="14">
-        <f t="shared" ref="B7:B12" si="1">B6+D6*1024</f>
-        <v>36864</v>
+        <f t="shared" ref="B7:B12" si="2">B6+D6*1024</f>
+        <v>24576</v>
       </c>
       <c r="C7" s="15" t="str">
-        <f t="shared" ref="C7:C12" si="2">"0x"&amp;RIGHT("00000000"&amp;DEC2HEX(B7),8)</f>
-        <v>0x00009000</v>
+        <f t="shared" si="0"/>
+        <v>0x00006000</v>
       </c>
       <c r="D7" s="15">
         <v>4</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1526,20 +1520,20 @@
         <v>10</v>
       </c>
       <c r="B8" s="19">
-        <f t="shared" si="1"/>
-        <v>40960</v>
+        <f t="shared" si="2"/>
+        <v>28672</v>
       </c>
       <c r="C8" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>0x0000A000</v>
+        <f t="shared" si="0"/>
+        <v>0x00007000</v>
       </c>
       <c r="D8" s="21">
-        <v>12</v>
+        <v>600</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="23">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1547,43 +1541,43 @@
         <v>11</v>
       </c>
       <c r="B9" s="19">
+        <f t="shared" si="2"/>
+        <v>643072</v>
+      </c>
+      <c r="C9" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>0x0009D000</v>
+      </c>
+      <c r="D9" s="21">
+        <v>356</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="23">
         <f t="shared" si="1"/>
-        <v>53248</v>
-      </c>
-      <c r="C9" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>0x0000D000</v>
-      </c>
-      <c r="D9" s="24">
-        <v>560</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23">
-        <f t="shared" si="0"/>
-        <v>140</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="19">
+        <f t="shared" si="2"/>
+        <v>1007616</v>
+      </c>
+      <c r="C10" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>0x000F6000</v>
+      </c>
+      <c r="D10" s="24">
         <v>12</v>
       </c>
-      <c r="B10" s="19">
+      <c r="E10" s="22"/>
+      <c r="F10" s="23">
         <f t="shared" si="1"/>
-        <v>626688</v>
-      </c>
-      <c r="C10" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>0x00099000</v>
-      </c>
-      <c r="D10" s="24">
-        <v>380</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="23">
-        <f t="shared" si="0"/>
-        <v>95</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1591,48 +1585,48 @@
         <v>14</v>
       </c>
       <c r="B11" s="19">
-        <f t="shared" si="1"/>
-        <v>1015808</v>
+        <f t="shared" si="2"/>
+        <v>1019904</v>
       </c>
       <c r="C11" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>0x000F8000</v>
-      </c>
-      <c r="D11" s="24">
+        <f t="shared" si="0"/>
+        <v>0x000F9000</v>
+      </c>
+      <c r="D11" s="21">
         <v>16</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" ht="14.25" spans="1:6">
       <c r="A12" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="19">
-        <f t="shared" si="1"/>
-        <v>1032192</v>
+        <f t="shared" si="2"/>
+        <v>1036288</v>
       </c>
       <c r="C12" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>0x000FC000</v>
+        <f t="shared" si="0"/>
+        <v>0x000FD000</v>
       </c>
       <c r="D12" s="26">
-        <f>B3-(D6+D7+D8+D9+D10+D11)</f>
-        <v>16</v>
+        <f>B3-(D6+D7+D10+D8+D9+D11)</f>
+        <v>12</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="28">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" ht="15.15"/>
-    <row r="15" ht="18.15" spans="1:2">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" ht="14.25"/>
+    <row r="15" ht="19.5" spans="1:2">
       <c r="A15" s="8" t="s">
         <v>1</v>
       </c>
@@ -1640,7 +1634,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="16" ht="15.15"/>
+    <row r="16" ht="14.25"/>
     <row r="17" spans="1:6">
       <c r="A17" s="10" t="s">
         <v>2</v>
@@ -1673,12 +1667,12 @@
         <v>0x00000000</v>
       </c>
       <c r="D18" s="15">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="17">
         <f t="shared" ref="F18:F24" si="3">D18/4</f>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1687,11 +1681,11 @@
       </c>
       <c r="B19" s="14">
         <f t="shared" ref="B19:B24" si="4">B18+D18*1024</f>
-        <v>36864</v>
+        <v>24576</v>
       </c>
       <c r="C19" s="15" t="str">
         <f t="shared" ref="C19:C24" si="5">"0x"&amp;RIGHT("00000000"&amp;DEC2HEX(B19),8)</f>
-        <v>0x00009000</v>
+        <v>0x00006000</v>
       </c>
       <c r="D19" s="15">
         <v>4</v>
@@ -1708,19 +1702,19 @@
       </c>
       <c r="B20" s="19">
         <f t="shared" si="4"/>
-        <v>40960</v>
+        <v>28672</v>
       </c>
       <c r="C20" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>0x0000A000</v>
+        <v>0x00007000</v>
       </c>
       <c r="D20" s="31">
-        <v>12</v>
+        <v>1200</v>
       </c>
       <c r="E20" s="32"/>
       <c r="F20" s="23">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1729,42 +1723,42 @@
       </c>
       <c r="B21" s="19">
         <f t="shared" si="4"/>
-        <v>53248</v>
+        <v>1257472</v>
       </c>
       <c r="C21" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>0x0000D000</v>
-      </c>
-      <c r="D21" s="24">
-        <v>1000</v>
-      </c>
-      <c r="E21" s="32"/>
+        <v>0x00133000</v>
+      </c>
+      <c r="D21" s="21">
+        <v>680</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>12</v>
+      </c>
       <c r="F21" s="23">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B22" s="19">
         <f t="shared" si="4"/>
-        <v>1077248</v>
+        <v>1953792</v>
       </c>
       <c r="C22" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>0x00107000</v>
-      </c>
-      <c r="D22" s="24">
-        <v>800</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>13</v>
-      </c>
+        <v>0x001DD000</v>
+      </c>
+      <c r="D22" s="33">
+        <v>12</v>
+      </c>
+      <c r="E22" s="32"/>
       <c r="F22" s="23">
         <f t="shared" si="3"/>
-        <v>200</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1773,13 +1767,13 @@
       </c>
       <c r="B23" s="19">
         <f t="shared" si="4"/>
-        <v>1896448</v>
+        <v>1966080</v>
       </c>
       <c r="C23" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>0x001CF000</v>
-      </c>
-      <c r="D23" s="24">
+        <v>0x001E0000</v>
+      </c>
+      <c r="D23" s="21">
         <v>16</v>
       </c>
       <c r="E23" s="32" t="s">
@@ -1790,30 +1784,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" ht="14.25" spans="1:6">
       <c r="A24" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B24" s="19">
         <f t="shared" si="4"/>
-        <v>1912832</v>
+        <v>1982464</v>
       </c>
       <c r="C24" s="20" t="str">
         <f t="shared" si="5"/>
-        <v>0x001D3000</v>
+        <v>0x001E4000</v>
       </c>
       <c r="D24" s="26">
         <f>B15-(D18+D19+D20+D21+D22+D23)</f>
-        <v>180</v>
-      </c>
-      <c r="E24" s="33"/>
+        <v>112</v>
+      </c>
+      <c r="E24" s="34"/>
       <c r="F24" s="28">
         <f t="shared" si="3"/>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" ht="15.15"/>
-    <row r="27" ht="18.15" spans="1:2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" ht="14.25"/>
+    <row r="27" ht="19.5" spans="1:2">
       <c r="A27" s="8" t="s">
         <v>1</v>
       </c>
@@ -1821,7 +1815,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="28" ht="15.15"/>
+    <row r="28" ht="14.25"/>
     <row r="29" spans="1:6">
       <c r="A29" s="10" t="s">
         <v>2</v>
@@ -1854,12 +1848,12 @@
         <v>0x00000000</v>
       </c>
       <c r="D30" s="15">
-        <v>36</v>
-      </c>
-      <c r="E30" s="16"/>
+        <v>24</v>
+      </c>
+      <c r="E30" s="30"/>
       <c r="F30" s="17">
-        <f>D30/4</f>
-        <v>9</v>
+        <f t="shared" ref="F30:F36" si="6">D30/4</f>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1867,82 +1861,85 @@
         <v>9</v>
       </c>
       <c r="B31" s="14">
-        <f t="shared" ref="B31:B36" si="6">B30+D30*1024</f>
-        <v>36864</v>
+        <f t="shared" ref="B31:B36" si="7">B30+D30*1024</f>
+        <v>24576</v>
       </c>
       <c r="C31" s="15" t="str">
-        <f t="shared" ref="C31:C36" si="7">"0x"&amp;RIGHT("00000000"&amp;DEC2HEX(B31),8)</f>
-        <v>0x00009000</v>
+        <f t="shared" ref="C31:C36" si="8">"0x"&amp;RIGHT("00000000"&amp;DEC2HEX(B31),8)</f>
+        <v>0x00006000</v>
       </c>
       <c r="D31" s="15">
         <v>4</v>
       </c>
-      <c r="E31" s="16"/>
+      <c r="E31" s="30"/>
       <c r="F31" s="17">
-        <f>D31/4</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="35">
+        <f t="shared" si="7"/>
+        <v>28672</v>
+      </c>
+      <c r="C32" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>0x00007000</v>
+      </c>
+      <c r="D32" s="31">
+        <v>2300</v>
+      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="36">
         <f t="shared" si="6"/>
-        <v>40960</v>
-      </c>
-      <c r="C32" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>0x0000A000</v>
-      </c>
-      <c r="D32" s="36">
-        <v>12</v>
-      </c>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
+        <v>575</v>
+      </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B33" s="35">
+        <f t="shared" si="7"/>
+        <v>2383872</v>
+      </c>
+      <c r="C33" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>0x00246000</v>
+      </c>
+      <c r="D33" s="21">
+        <v>1600</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="23">
         <f t="shared" si="6"/>
-        <v>53248</v>
-      </c>
-      <c r="C33" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>0x0000D000</v>
-      </c>
-      <c r="D33" s="24">
-        <v>2300</v>
-      </c>
-      <c r="E33" s="22"/>
-      <c r="F33" s="23">
-        <f>D33/4</f>
-        <v>575</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="35">
+        <f t="shared" si="7"/>
+        <v>4022272</v>
+      </c>
+      <c r="C34" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>0x003D6000</v>
+      </c>
+      <c r="D34" s="33">
         <v>12</v>
       </c>
-      <c r="B34" s="35">
+      <c r="E34" s="32"/>
+      <c r="F34" s="23">
         <f t="shared" si="6"/>
-        <v>2408448</v>
-      </c>
-      <c r="C34" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>0x0024C000</v>
-      </c>
-      <c r="D34" s="24">
-        <v>1600</v>
-      </c>
-      <c r="E34" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="23">
-        <f>D34/4</f>
-        <v>400</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1950,44 +1947,44 @@
         <v>14</v>
       </c>
       <c r="B35" s="35">
+        <f t="shared" si="7"/>
+        <v>4034560</v>
+      </c>
+      <c r="C35" s="20" t="str">
+        <f t="shared" si="8"/>
+        <v>0x003D9000</v>
+      </c>
+      <c r="D35" s="21">
+        <v>16</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="23">
         <f t="shared" si="6"/>
-        <v>4046848</v>
-      </c>
-      <c r="C35" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>0x003DC000</v>
-      </c>
-      <c r="D35" s="24">
-        <v>16</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="23">
-        <f>D35/4</f>
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" ht="14.25" spans="1:6">
       <c r="A36" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="39">
-        <f t="shared" si="6"/>
-        <v>4063232</v>
+      <c r="B36" s="37">
+        <f t="shared" si="7"/>
+        <v>4050944</v>
       </c>
       <c r="C36" s="20" t="str">
-        <f t="shared" si="7"/>
-        <v>0x003E0000</v>
+        <f t="shared" si="8"/>
+        <v>0x003DD000</v>
       </c>
       <c r="D36" s="26">
         <f>B27-(D30+D31+D32+D33+D34+D35)</f>
-        <v>128</v>
-      </c>
-      <c r="E36" s="27"/>
+        <v>140</v>
+      </c>
+      <c r="E36" s="34"/>
       <c r="F36" s="28">
-        <f>D36/4</f>
-        <v>32</v>
+        <f t="shared" si="6"/>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2009,7 +2006,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2026,7 +2023,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>